<commit_message>
moved impulse response to convolve
</commit_message>
<xml_diff>
--- a/datasets/Winawer2016_data.xlsx
+++ b/datasets/Winawer2016_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="17">
   <si>
     <t>Paper</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">  NaN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NaN</t>
   </si>
   <si>
     <t xml:space="preserve">   NaN</t>
@@ -419,8 +416,8 @@
   <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K86" sqref="K86:K103"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,7 +458,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>12</v>
@@ -492,8 +489,8 @@
       <c r="H2" s="5">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
+      <c r="I2" s="4">
+        <v>-1000</v>
       </c>
       <c r="J2" s="5">
         <v>20.230499999999999</v>
@@ -530,8 +527,8 @@
       <c r="H3" s="5">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
+      <c r="I3" s="4">
+        <v>-1000</v>
       </c>
       <c r="J3" s="5">
         <v>4.6905000000000001</v>
@@ -568,8 +565,8 @@
       <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>15</v>
+      <c r="I4" s="4">
+        <v>-1000</v>
       </c>
       <c r="J4" s="5">
         <v>73.634</v>
@@ -606,8 +603,8 @@
       <c r="H5" s="5">
         <v>2</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>15</v>
+      <c r="I5" s="4">
+        <v>-1000</v>
       </c>
       <c r="J5" s="5">
         <v>14.000999999999999</v>
@@ -644,8 +641,8 @@
       <c r="H6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>15</v>
+      <c r="I6" s="4">
+        <v>-1000</v>
       </c>
       <c r="J6" s="5">
         <v>2.8681000000000001</v>
@@ -682,8 +679,8 @@
       <c r="H7" s="5">
         <v>2</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>15</v>
+      <c r="I7" s="4">
+        <v>-1000</v>
       </c>
       <c r="J7" s="5">
         <v>0.17519999999999999</v>
@@ -720,8 +717,8 @@
       <c r="H8" s="5">
         <v>5</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>15</v>
+      <c r="I8" s="4">
+        <v>-1000</v>
       </c>
       <c r="J8" s="5">
         <v>8.9921000000000006</v>
@@ -758,8 +755,8 @@
       <c r="H9" s="5">
         <v>2</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>15</v>
+      <c r="I9" s="4">
+        <v>-1000</v>
       </c>
       <c r="J9" s="5">
         <v>7.5922999999999998</v>
@@ -796,8 +793,8 @@
       <c r="H10" s="5">
         <v>2</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>15</v>
+      <c r="I10" s="4">
+        <v>-1000</v>
       </c>
       <c r="J10" s="5">
         <v>12.1075</v>
@@ -834,8 +831,8 @@
       <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>15</v>
+      <c r="I11" s="4">
+        <v>-1000</v>
       </c>
       <c r="J11" s="5">
         <v>1.6354</v>
@@ -872,8 +869,8 @@
       <c r="H12" s="5">
         <v>2</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>15</v>
+      <c r="I12" s="4">
+        <v>-1000</v>
       </c>
       <c r="J12" s="5">
         <v>44.887500000000003</v>
@@ -910,8 +907,8 @@
       <c r="H13" s="5">
         <v>5</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>15</v>
+      <c r="I13" s="4">
+        <v>-1000</v>
       </c>
       <c r="J13" s="5">
         <v>81.242000000000004</v>
@@ -948,8 +945,8 @@
       <c r="H14" s="5">
         <v>5</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>15</v>
+      <c r="I14" s="4">
+        <v>-1000</v>
       </c>
       <c r="J14" s="5">
         <v>11.581200000000001</v>
@@ -986,8 +983,8 @@
       <c r="H15" s="5">
         <v>2</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>15</v>
+      <c r="I15" s="4">
+        <v>-1000</v>
       </c>
       <c r="J15" s="5">
         <v>3.6126999999999998</v>
@@ -1024,8 +1021,8 @@
       <c r="H16" s="5">
         <v>5</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>15</v>
+      <c r="I16" s="4">
+        <v>-1000</v>
       </c>
       <c r="J16" s="5">
         <v>44.269300000000001</v>
@@ -1062,8 +1059,8 @@
       <c r="H17" s="5">
         <v>5</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>15</v>
+      <c r="I17" s="4">
+        <v>-1000</v>
       </c>
       <c r="J17" s="5">
         <v>75.5505</v>
@@ -1100,8 +1097,8 @@
       <c r="H18" s="5">
         <v>2</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>15</v>
+      <c r="I18" s="4">
+        <v>-1000</v>
       </c>
       <c r="J18" s="5">
         <v>43.511899999999997</v>
@@ -1138,8 +1135,8 @@
       <c r="H19" s="5">
         <v>5</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>15</v>
+      <c r="I19" s="4">
+        <v>-1000</v>
       </c>
       <c r="J19" s="5">
         <v>145.4306</v>
@@ -1176,8 +1173,8 @@
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>15</v>
+      <c r="I20" s="4">
+        <v>0</v>
       </c>
       <c r="J20">
         <v>48.3367</v>
@@ -1328,8 +1325,8 @@
       <c r="H24">
         <v>4</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>16</v>
+      <c r="I24" s="4">
+        <v>0</v>
       </c>
       <c r="J24">
         <v>27.741700000000002</v>
@@ -1366,8 +1363,8 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>16</v>
+      <c r="I25" s="4">
+        <v>0</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
@@ -1442,8 +1439,8 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>16</v>
+      <c r="I27" s="4">
+        <v>0</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -1708,8 +1705,8 @@
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>16</v>
+      <c r="I34" s="4">
+        <v>0</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -1898,8 +1895,8 @@
       <c r="H39">
         <v>0</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>16</v>
+      <c r="I39" s="4">
+        <v>0</v>
       </c>
       <c r="J39" t="s">
         <v>11</v>
@@ -2126,8 +2123,8 @@
       <c r="H45" s="5">
         <v>0</v>
       </c>
-      <c r="I45" s="6" t="s">
-        <v>15</v>
+      <c r="I45" s="4">
+        <v>0</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>13</v>
@@ -2354,8 +2351,8 @@
       <c r="H51" s="5">
         <v>0</v>
       </c>
-      <c r="I51" s="6" t="s">
-        <v>16</v>
+      <c r="I51" s="4">
+        <v>0</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>11</v>
@@ -2468,8 +2465,8 @@
       <c r="H54" s="5">
         <v>0</v>
       </c>
-      <c r="I54" s="6" t="s">
-        <v>16</v>
+      <c r="I54" s="4">
+        <v>0</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>11</v>
@@ -2772,8 +2769,8 @@
       <c r="H62" s="5">
         <v>0</v>
       </c>
-      <c r="I62" s="6" t="s">
-        <v>16</v>
+      <c r="I62" s="4">
+        <v>0</v>
       </c>
       <c r="J62" s="5" t="s">
         <v>11</v>
@@ -2810,8 +2807,8 @@
       <c r="H63" s="5">
         <v>0</v>
       </c>
-      <c r="I63" s="6" t="s">
-        <v>16</v>
+      <c r="I63" s="4">
+        <v>0</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>11</v>
@@ -2924,8 +2921,8 @@
       <c r="H66">
         <v>2</v>
       </c>
-      <c r="I66" s="4" t="s">
-        <v>16</v>
+      <c r="I66" s="4">
+        <v>-1000</v>
       </c>
       <c r="J66">
         <v>9.3835999999999995</v>
@@ -2962,8 +2959,8 @@
       <c r="H67">
         <v>2</v>
       </c>
-      <c r="I67" s="4" t="s">
-        <v>16</v>
+      <c r="I67" s="4">
+        <v>-1000</v>
       </c>
       <c r="J67">
         <v>4.4668999999999999</v>
@@ -3000,8 +2997,8 @@
       <c r="H68">
         <v>2</v>
       </c>
-      <c r="I68" s="4" t="s">
-        <v>16</v>
+      <c r="I68" s="4">
+        <v>-1000</v>
       </c>
       <c r="J68">
         <v>1.194</v>
@@ -3038,8 +3035,8 @@
       <c r="H69">
         <v>2</v>
       </c>
-      <c r="I69" s="4" t="s">
-        <v>16</v>
+      <c r="I69" s="4">
+        <v>-1000</v>
       </c>
       <c r="J69">
         <v>7.8013000000000003</v>
@@ -3076,8 +3073,8 @@
       <c r="H70">
         <v>2</v>
       </c>
-      <c r="I70" s="4" t="s">
-        <v>16</v>
+      <c r="I70" s="4">
+        <v>-1000</v>
       </c>
       <c r="J70">
         <v>18.8903</v>
@@ -3114,8 +3111,8 @@
       <c r="H71">
         <v>2</v>
       </c>
-      <c r="I71" s="4" t="s">
-        <v>16</v>
+      <c r="I71" s="4">
+        <v>-1000</v>
       </c>
       <c r="J71">
         <v>1.3933</v>
@@ -3152,8 +3149,8 @@
       <c r="H72">
         <v>2</v>
       </c>
-      <c r="I72" s="4" t="s">
-        <v>16</v>
+      <c r="I72" s="4">
+        <v>-1000</v>
       </c>
       <c r="J72">
         <v>12.3691</v>
@@ -3190,8 +3187,8 @@
       <c r="H73">
         <v>2</v>
       </c>
-      <c r="I73" s="4" t="s">
-        <v>16</v>
+      <c r="I73" s="4">
+        <v>-1000</v>
       </c>
       <c r="J73">
         <v>2.8965999999999998</v>
@@ -3228,8 +3225,8 @@
       <c r="H74">
         <v>0.2</v>
       </c>
-      <c r="I74" s="4" t="s">
-        <v>16</v>
+      <c r="I74" s="4">
+        <v>-1000</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -3266,8 +3263,8 @@
       <c r="H75">
         <v>2</v>
       </c>
-      <c r="I75" s="4" t="s">
-        <v>16</v>
+      <c r="I75" s="4">
+        <v>-1000</v>
       </c>
       <c r="J75">
         <v>16.726400000000002</v>
@@ -3304,8 +3301,8 @@
       <c r="H76">
         <v>5</v>
       </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
+      <c r="I76" s="4">
+        <v>-1000</v>
       </c>
       <c r="J76">
         <v>2.8871000000000002</v>
@@ -3342,8 +3339,8 @@
       <c r="H77">
         <v>5</v>
       </c>
-      <c r="I77" s="4" t="s">
-        <v>16</v>
+      <c r="I77" s="4">
+        <v>-1000</v>
       </c>
       <c r="J77">
         <v>23.225000000000001</v>
@@ -3380,8 +3377,8 @@
       <c r="H78">
         <v>5</v>
       </c>
-      <c r="I78" s="4" t="s">
-        <v>16</v>
+      <c r="I78" s="4">
+        <v>-1000</v>
       </c>
       <c r="J78">
         <v>47.206200000000003</v>
@@ -3418,8 +3415,8 @@
       <c r="H79">
         <v>5</v>
       </c>
-      <c r="I79" s="4" t="s">
-        <v>16</v>
+      <c r="I79" s="4">
+        <v>-1000</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -3456,8 +3453,8 @@
       <c r="H80">
         <v>5</v>
       </c>
-      <c r="I80" s="4" t="s">
-        <v>16</v>
+      <c r="I80" s="4">
+        <v>-1000</v>
       </c>
       <c r="J80">
         <v>70.341999999999999</v>
@@ -3494,8 +3491,8 @@
       <c r="H81">
         <v>5</v>
       </c>
-      <c r="I81" s="4" t="s">
-        <v>16</v>
+      <c r="I81" s="4">
+        <v>-1000</v>
       </c>
       <c r="J81">
         <v>1.0106999999999999</v>
@@ -3532,8 +3529,8 @@
       <c r="H82">
         <v>5</v>
       </c>
-      <c r="I82" s="4" t="s">
-        <v>16</v>
+      <c r="I82" s="4">
+        <v>-1000</v>
       </c>
       <c r="J82">
         <v>56.619</v>
@@ -3570,8 +3567,8 @@
       <c r="H83">
         <v>5</v>
       </c>
-      <c r="I83" s="4" t="s">
-        <v>16</v>
+      <c r="I83" s="4">
+        <v>-1000</v>
       </c>
       <c r="J83">
         <v>43.239699999999999</v>
@@ -3608,8 +3605,8 @@
       <c r="H84">
         <v>5</v>
       </c>
-      <c r="I84" s="4" t="s">
-        <v>16</v>
+      <c r="I84" s="4">
+        <v>-1000</v>
       </c>
       <c r="J84">
         <v>0.90349999999999997</v>
@@ -3646,8 +3643,8 @@
       <c r="H85">
         <v>5</v>
       </c>
-      <c r="I85" s="4" t="s">
-        <v>16</v>
+      <c r="I85" s="4">
+        <v>-1000</v>
       </c>
       <c r="J85">
         <v>70.197299999999998</v>
@@ -3684,14 +3681,14 @@
       <c r="H86" s="5">
         <v>1</v>
       </c>
-      <c r="I86" s="6" t="s">
-        <v>14</v>
+      <c r="I86" s="4">
+        <v>0</v>
       </c>
       <c r="J86" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L86" s="5">
         <v>10</v>
@@ -3760,8 +3757,8 @@
       <c r="H88" s="5">
         <v>3</v>
       </c>
-      <c r="I88" s="6" t="s">
-        <v>16</v>
+      <c r="I88" s="4">
+        <v>0</v>
       </c>
       <c r="J88" s="5" t="s">
         <v>11</v>
@@ -3798,8 +3795,8 @@
       <c r="H89" s="5">
         <v>3</v>
       </c>
-      <c r="I89" s="6" t="s">
-        <v>16</v>
+      <c r="I89" s="4">
+        <v>0</v>
       </c>
       <c r="J89" s="5" t="s">
         <v>11</v>
@@ -3836,8 +3833,8 @@
       <c r="H90" s="5">
         <v>3</v>
       </c>
-      <c r="I90" s="6" t="s">
-        <v>16</v>
+      <c r="I90" s="4">
+        <v>0</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>11</v>
@@ -3874,8 +3871,8 @@
       <c r="H91" s="5">
         <v>0</v>
       </c>
-      <c r="I91" s="6" t="s">
-        <v>16</v>
+      <c r="I91" s="4">
+        <v>0</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>11</v>
@@ -3912,8 +3909,8 @@
       <c r="H92" s="5">
         <v>0</v>
       </c>
-      <c r="I92" s="6" t="s">
-        <v>16</v>
+      <c r="I92" s="4">
+        <v>0</v>
       </c>
       <c r="J92" s="5" t="s">
         <v>11</v>
@@ -4026,8 +4023,8 @@
       <c r="H95" s="5">
         <v>0</v>
       </c>
-      <c r="I95" s="6" t="s">
-        <v>16</v>
+      <c r="I95" s="4">
+        <v>0</v>
       </c>
       <c r="J95" s="5" t="s">
         <v>11</v>
@@ -4178,8 +4175,8 @@
       <c r="H99" s="5">
         <v>5</v>
       </c>
-      <c r="I99" s="6" t="s">
-        <v>16</v>
+      <c r="I99" s="4">
+        <v>0</v>
       </c>
       <c r="J99" s="5" t="s">
         <v>11</v>
@@ -4216,8 +4213,8 @@
       <c r="H100" s="5">
         <v>0</v>
       </c>
-      <c r="I100" s="6" t="s">
-        <v>16</v>
+      <c r="I100" s="4">
+        <v>0</v>
       </c>
       <c r="J100" s="5" t="s">
         <v>11</v>

</xml_diff>